<commit_message>
changed probe convert table
</commit_message>
<xml_diff>
--- a/ProbeTypeConvert.xlsx
+++ b/ProbeTypeConvert.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fanwu/Documents/Impedance_sort/Impedance_sort/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7E293E-C429-2A44-9945-77E36418B4C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE75520-7A6B-FE4F-B039-D01EE1FD0964}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="980" windowWidth="27640" windowHeight="15520" xr2:uid="{8A82474E-F1B0-3647-B562-AD4C1AD99706}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
   <si>
     <t>16-1-6mm</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>CNT</t>
+  </si>
+  <si>
+    <t>H10</t>
   </si>
 </sst>
 </file>
@@ -561,7 +564,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -798,7 +801,7 @@
         <v>46</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>